<commit_message>
[+] room create cost .config
</commit_message>
<xml_diff>
--- a/tools/xlsx2json/excel/GameConfig.xlsx
+++ b/tools/xlsx2json/excel/GameConfig.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24195" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24195" windowHeight="12870" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RoomConfig" sheetId="3" r:id="rId1"/>
+    <sheet name="RoomCreateCost" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>app_name</t>
   </si>
@@ -182,6 +183,42 @@
   </si>
   <si>
     <t>匹配规则 private/normal/challenge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost_id#id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game_cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏局</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -528,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -726,4 +763,109 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>5001</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>5001</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>5001</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>